<commit_message>
Adding APIs and inference provides
</commit_message>
<xml_diff>
--- a/Groq_Chatbot/models_list.xlsx
+++ b/Groq_Chatbot/models_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,16 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>whisper-large-v3</t>
+          <t>allam-2-7b</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -483,16 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>meta-llama/llama-prompt-guard-2-86m</t>
+          <t>compound-beta</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -503,16 +503,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>playai-tts</t>
+          <t>compound-beta-mini</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -523,7 +523,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>llama3-8b-8192</t>
+          <t>deepseek-r1-distill-llama-70b</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>llama3-70b-8192</t>
+          <t>gemma2-9b-it</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -583,16 +583,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>playai-tts-arabic</t>
+          <t>llama-3.1-8b-instant</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -603,7 +603,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>compound-beta-mini</t>
+          <t>llama-3.3-70b-versatile</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>openai/gpt-oss-20b</t>
+          <t>llama3-70b-8192</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -643,7 +643,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>openai/gpt-oss-120b</t>
+          <t>llama3-8b-8192</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -663,16 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>meta-llama/llama-prompt-guard-2-22m</t>
+          <t>meta-llama/llama-4-maverick-17b-128e-instruct</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -683,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>deepseek-r1-distill-llama-70b</t>
+          <t>meta-llama/llama-4-scout-17b-16e-instruct</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -703,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>qwen/qwen3-32b</t>
+          <t>meta-llama/llama-guard-4-12b</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -723,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>compound-beta</t>
+          <t>meta-llama/llama-prompt-guard-2-22m</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -743,7 +743,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>llama-3.3-70b-versatile</t>
+          <t>meta-llama/llama-prompt-guard-2-86m</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -763,16 +763,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>whisper-large-v3-turbo</t>
+          <t>moonshotai/kimi-k2-instruct</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -783,7 +783,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>llama-3.1-8b-instant</t>
+          <t>openai/gpt-oss-120b</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -803,7 +803,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>meta-llama/llama-4-maverick-17b-128e-instruct</t>
+          <t>openai/gpt-oss-20b</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -823,16 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>meta-llama/llama-4-scout-17b-16e-instruct</t>
+          <t>playai-tts</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>audio</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
@@ -843,16 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>moonshotai/kimi-k2-instruct</t>
+          <t>playai-tts-arabic</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>audio</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -863,16 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>meta-llama/llama-guard-4-12b</t>
+          <t>qwen/qwen3-32b</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -883,16 +883,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>gemma2-9b-it</t>
+          <t>whisper-large-v3</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>audio</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -903,16 +903,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>allam-2-7b</t>
+          <t>whisper-large-v3-turbo</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>audio</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -923,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>mistral-medium-2505</t>
+          <t>codestral-2411-rc5</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -943,12 +943,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>mistral-large-latest</t>
+          <t>codestral-2412</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -963,7 +963,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>mistral-medium-2508</t>
+          <t>codestral-2501</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -983,16 +983,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>mistral-medium-latest</t>
+          <t>codestral-2508</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
@@ -1003,16 +1003,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>mistral-medium</t>
+          <t>codestral-embed</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -1023,16 +1023,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ministral-3b-2410</t>
+          <t>codestral-embed-2505</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -1043,16 +1043,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ministral-3b-latest</t>
+          <t>codestral-latest</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ministral-8b-2410</t>
+          <t>devstral-medium-2507</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -1083,16 +1083,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ministral-8b-latest</t>
+          <t>devstral-medium-latest</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>open-mistral-7b</t>
+          <t>devstral-small-2505</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>mistral-tiny</t>
+          <t>devstral-small-2507</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1143,16 +1143,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>mistral-tiny-2312</t>
+          <t>devstral-small-latest</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>open-mistral-nemo</t>
+          <t>magistral-medium-2506</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1183,16 +1183,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>open-mistral-nemo-2407</t>
+          <t>magistral-medium-2507</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -1203,16 +1203,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>mistral-tiny-2407</t>
+          <t>magistral-medium-latest</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>mistral-tiny-latest</t>
+          <t>magistral-small-2506</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>open-mixtral-8x7b</t>
+          <t>magistral-small-2507</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>mistral-small</t>
+          <t>magistral-small-latest</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>mistral-small-2312</t>
+          <t>ministral-3b-2410</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>open-mixtral-8x22b</t>
+          <t>ministral-3b-latest</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>open-mixtral-8x22b-2404</t>
+          <t>ministral-8b-2410</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>mistral-small-2409</t>
+          <t>ministral-8b-latest</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>mistral-large-2407</t>
+          <t>mistral-embed</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>mistral-large-2411</t>
+          <t>mistral-large-2407</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1403,16 +1403,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>pixtral-large-2411</t>
+          <t>mistral-large-2411</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50">
@@ -1423,12 +1423,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>pixtral-large-latest</t>
+          <t>mistral-large-latest</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -1463,16 +1463,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>codestral-2501</t>
+          <t>mistral-medium</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53">
@@ -1483,16 +1483,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>codestral-2412</t>
+          <t>mistral-medium-2505</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
@@ -1503,16 +1503,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>codestral-2411-rc5</t>
+          <t>mistral-medium-2508</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55">
@@ -1523,16 +1523,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>codestral-2508</t>
+          <t>mistral-medium-latest</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
@@ -1543,16 +1543,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>codestral-latest</t>
+          <t>mistral-moderation-2411</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>devstral-small-2505</t>
+          <t>mistral-moderation-latest</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58">
@@ -1583,16 +1583,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>devstral-small-2507</t>
+          <t>mistral-ocr-2503</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>vision</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59">
@@ -1603,16 +1603,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>devstral-small-latest</t>
+          <t>mistral-ocr-2505</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>vision</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>devstral-medium-2507</t>
+          <t>mistral-ocr-latest</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>vision</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1643,16 +1643,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>devstral-medium-latest</t>
+          <t>mistral-saba-2502</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
@@ -1663,16 +1663,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>pixtral-12b-2409</t>
+          <t>mistral-saba-latest</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63">
@@ -1683,16 +1683,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>pixtral-12b</t>
+          <t>mistral-small</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -1703,16 +1703,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>pixtral-12b-latest</t>
+          <t>mistral-small-2312</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>mistral-small-2501</t>
+          <t>mistral-small-2409</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -1743,16 +1743,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>mistral-small-2503</t>
+          <t>mistral-small-2501</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
@@ -1763,16 +1763,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>mistral-small-2506</t>
+          <t>mistral-small-2503</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>mistral-small-latest</t>
+          <t>mistral-small-2506</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>mistral-saba-2502</t>
+          <t>mistral-small-latest</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>mistral-saba-latest</t>
+          <t>mistral-tiny</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>magistral-medium-2506</t>
+          <t>mistral-tiny-2312</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -1863,16 +1863,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>magistral-medium-2507</t>
+          <t>mistral-tiny-2407</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
@@ -1883,16 +1883,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>magistral-medium-latest</t>
+          <t>mistral-tiny-latest</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>magistral-small-2506</t>
+          <t>open-mistral-7b</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>magistral-small-2507</t>
+          <t>open-mistral-nemo</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>magistral-small-latest</t>
+          <t>open-mistral-nemo-2407</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77">
@@ -1963,12 +1963,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>voxtral-mini-2507</t>
+          <t>open-mixtral-8x22b</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -1983,16 +1983,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>voxtral-mini-latest</t>
+          <t>open-mixtral-8x22b-2404</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79">
@@ -2003,12 +2003,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>voxtral-small-2507</t>
+          <t>open-mixtral-8x7b</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>multimodal</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>voxtral-small-latest</t>
+          <t>pixtral-12b</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2043,16 +2043,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>mistral-embed</t>
+          <t>pixtral-12b-2409</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
@@ -2063,16 +2063,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>codestral-embed</t>
+          <t>pixtral-12b-latest</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -2083,16 +2083,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>codestral-embed-2505</t>
+          <t>pixtral-large-2411</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>coding</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84">
@@ -2103,16 +2103,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>mistral-moderation-2411</t>
+          <t>pixtral-large-latest</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
@@ -2123,16 +2123,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>mistral-moderation-latest</t>
+          <t>voxtral-mini-2507</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86">
@@ -2143,16 +2143,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>mistral-ocr-2503</t>
+          <t>voxtral-mini-latest</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>vision</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87">
@@ -2163,16 +2163,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>mistral-ocr-2505</t>
+          <t>voxtral-mini-transcribe-2507</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>vision</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88">
@@ -2183,12 +2183,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>mistral-ocr-latest</t>
+          <t>voxtral-small-2507</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>vision</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2203,56 +2203,16 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>voxtral-mini-transcribe-2507</t>
+          <t>voxtral-small-latest</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>audio</t>
+          <t>multimodal</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Mistral</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>voxtral-mini-2507</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>multimodal</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Mistral</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>voxtral-mini-latest</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>multimodal</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>